<commit_message>
updated SIT crosswalk with minor fixes and added a crosswalk for perente et al 2024 dominant grassland types
</commit_message>
<xml_diff>
--- a/sisepuede/ref/data_crosswalks/sisepuede_fields_to_epa_state_inventory_tool_emissions_map.xlsx
+++ b/sisepuede/ref/data_crosswalks/sisepuede_fields_to_epa_state_inventory_tool_emissions_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/Documents/Projects/Louisiana/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/data_crosswalks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EA9FEB-0229-354D-ABF1-AA56701125F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0729AAE4-B8E7-9B44-9C56-DCFF2A289AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="760" windowWidth="33420" windowHeight="18280" activeTab="1" xr2:uid="{9DBDAEDA-F5AA-E443-9947-E206192A213F}"/>
+    <workbookView xWindow="4420" yWindow="760" windowWidth="33420" windowHeight="18280" activeTab="1" xr2:uid="{9DBDAEDA-F5AA-E443-9947-E206192A213F}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -385,9 +385,6 @@
     <t>Industrial</t>
   </si>
   <si>
-    <t>15|17|18|19</t>
-  </si>
-  <si>
     <t>Coal|Natural Gas|Other|Petroleum</t>
   </si>
   <si>
@@ -1515,6 +1512,9 @@
       </rPr>
       <t xml:space="preserve">O </t>
     </r>
+  </si>
+  <si>
+    <t>15|16|17|18</t>
   </si>
 </sst>
 </file>
@@ -1617,32 +1617,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1996,10 +1995,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2007,26 +2006,26 @@
         <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
         <v>122</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2034,15 +2033,15 @@
         <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" t="s">
         <v>126</v>
-      </c>
-      <c r="C6" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2054,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9645CE76-D122-B846-99B1-A3A394E64618}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2107,21 +2106,21 @@
         <v>74</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -2133,16 +2132,16 @@
         <v>17</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>178</v>
+        <v>171</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="L2" s="4">
         <v>35</v>
@@ -2151,16 +2150,16 @@
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -2172,16 +2171,16 @@
         <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="K3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>179</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="L3" s="4">
         <v>36</v>
@@ -2190,16 +2189,16 @@
     </row>
     <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -2211,16 +2210,16 @@
         <v>3</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>179</v>
+        <v>171</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="L4" s="4">
         <v>40</v>
@@ -2229,16 +2228,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -2268,16 +2267,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -2307,16 +2306,16 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -2346,16 +2345,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -2385,16 +2384,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -2424,16 +2423,16 @@
     </row>
     <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -2445,16 +2444,16 @@
         <v>3</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="K10" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>205</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="L10" s="4">
         <v>46</v>
@@ -2463,16 +2462,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -2502,16 +2501,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -2541,16 +2540,16 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
@@ -2603,13 +2602,13 @@
       <c r="H14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>294</v>
+      <c r="I14" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="8" t="s">
         <v>23</v>
       </c>
       <c r="L14" s="4">
@@ -2642,13 +2641,13 @@
       <c r="H15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>31</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="8" t="s">
         <v>21</v>
       </c>
       <c r="L15" s="4">
@@ -2681,13 +2680,13 @@
       <c r="H16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>294</v>
+      <c r="I16" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="8" t="s">
         <v>12</v>
       </c>
       <c r="L16" s="4">
@@ -2720,13 +2719,13 @@
       <c r="H17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>294</v>
+      <c r="I17" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" s="8" t="s">
         <v>28</v>
       </c>
       <c r="L17" s="4">
@@ -2759,14 +2758,14 @@
       <c r="H18" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>295</v>
+      <c r="I18" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="9" t="s">
-        <v>296</v>
+      <c r="K18" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="L18" s="4">
         <v>9</v>
@@ -3149,13 +3148,13 @@
       <c r="H28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="8" t="s">
-        <v>294</v>
+      <c r="I28" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" s="8" t="s">
         <v>33</v>
       </c>
       <c r="L28" s="4">
@@ -3188,13 +3187,13 @@
       <c r="H29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>294</v>
+      <c r="I29" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L29" s="4">
@@ -3227,8 +3226,8 @@
       <c r="H30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>297</v>
+      <c r="I30" s="9" t="s">
+        <v>296</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>20</v>
@@ -3264,8 +3263,8 @@
       <c r="H31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>294</v>
+      <c r="I31" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>19</v>
@@ -3301,8 +3300,8 @@
       <c r="H32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>298</v>
+      <c r="I32" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>12</v>
@@ -3338,8 +3337,8 @@
       <c r="H33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>294</v>
+      <c r="I33" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>12</v>
@@ -3358,10 +3357,10 @@
         <v>9</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="E34" s="3">
         <v>1</v>
@@ -3375,17 +3374,17 @@
       <c r="H34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>294</v>
+      <c r="I34" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>114</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>115</v>
+        <v>310</v>
       </c>
       <c r="M34" s="3"/>
     </row>
@@ -3396,7 +3395,7 @@
       <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -3414,11 +3413,11 @@
       <c r="H35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I35" s="8" t="s">
-        <v>294</v>
+      <c r="I35" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J35" s="3"/>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="8" t="s">
         <v>33</v>
       </c>
       <c r="L35" s="4">
@@ -3451,8 +3450,8 @@
       <c r="H36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I36" s="8" t="s">
-        <v>294</v>
+      <c r="I36" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3" t="s">
@@ -3465,16 +3464,16 @@
     </row>
     <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -3486,16 +3485,16 @@
         <v>14</v>
       </c>
       <c r="H37" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="J37" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>247</v>
+      <c r="K37" s="10" t="s">
+        <v>246</v>
       </c>
       <c r="L37" s="4">
         <v>27</v>
@@ -3504,16 +3503,16 @@
     </row>
     <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -3525,34 +3524,34 @@
         <v>14</v>
       </c>
       <c r="H38" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="J38" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="J38" s="9" t="s">
+      <c r="K38" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="L38" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>241</v>
       </c>
       <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
@@ -3582,16 +3581,16 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
@@ -3621,16 +3620,16 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
@@ -3660,16 +3659,16 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
@@ -3933,16 +3932,16 @@
     </row>
     <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E49" s="3">
         <v>1</v>
@@ -3956,32 +3955,32 @@
       <c r="H49" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I49" s="8" t="s">
-        <v>295</v>
+      <c r="I49" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="E50" s="3">
         <v>1</v>
@@ -3995,14 +3994,14 @@
       <c r="H50" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I50" s="8" t="s">
-        <v>295</v>
+      <c r="I50" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K50" s="9" t="s">
-        <v>139</v>
+      <c r="K50" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="L50" s="4">
         <v>5</v>
@@ -4011,16 +4010,16 @@
     </row>
     <row r="51" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E51" s="3">
         <v>1</v>
@@ -4034,14 +4033,14 @@
       <c r="H51" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I51" s="8" t="s">
-        <v>295</v>
+      <c r="I51" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K51" s="9" t="s">
-        <v>145</v>
+      <c r="K51" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="L51" s="4">
         <v>8</v>
@@ -4050,16 +4049,16 @@
     </row>
     <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
@@ -4073,14 +4072,14 @@
       <c r="H52" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I52" s="8" t="s">
-        <v>295</v>
+      <c r="I52" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K52" s="9" t="s">
-        <v>143</v>
+      <c r="K52" s="8" t="s">
+        <v>142</v>
       </c>
       <c r="L52" s="4">
         <v>6</v>
@@ -4089,16 +4088,16 @@
     </row>
     <row r="53" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -4112,32 +4111,32 @@
       <c r="H53" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I53" s="8" t="s">
-        <v>295</v>
+      <c r="I53" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K53" s="9" t="s">
-        <v>301</v>
+      <c r="K53" s="8" t="s">
+        <v>300</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M53" s="3"/>
     </row>
     <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="E54" s="3">
         <v>1</v>
@@ -4151,32 +4150,32 @@
       <c r="H54" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I54" s="8" t="s">
-        <v>295</v>
+      <c r="I54" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K54" s="9" t="s">
+      <c r="K54" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="L54" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="L54" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="M54" s="3"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="E55" s="3">
         <v>0</v>
@@ -4206,16 +4205,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E56" s="3">
         <v>0</v>
@@ -4245,16 +4244,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
@@ -4284,16 +4283,16 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
@@ -4323,16 +4322,16 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E59" s="3">
         <v>0</v>
@@ -4362,16 +4361,16 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E60" s="3">
         <v>0</v>
@@ -4401,16 +4400,16 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E61" s="3">
         <v>0</v>
@@ -4440,16 +4439,16 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E62" s="3">
         <v>0</v>
@@ -4479,16 +4478,16 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E63" s="3">
         <v>0</v>
@@ -4518,16 +4517,16 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E64" s="3">
         <v>0</v>
@@ -4557,16 +4556,16 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E65" s="3">
         <v>0</v>
@@ -4596,16 +4595,16 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E66" s="3">
         <v>0</v>
@@ -4635,16 +4634,16 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E67" s="3">
         <v>0</v>
@@ -4674,16 +4673,16 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E68" s="3">
         <v>0</v>
@@ -4713,16 +4712,16 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E69" s="3">
         <v>0</v>
@@ -4752,16 +4751,16 @@
     </row>
     <row r="70" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E70" s="3">
         <v>1</v>
@@ -4773,15 +4772,15 @@
         <v>14</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="K70" s="11"/>
+        <v>251</v>
+      </c>
+      <c r="K70" s="10"/>
       <c r="L70" s="4">
         <v>40</v>
       </c>
@@ -4789,16 +4788,16 @@
     </row>
     <row r="71" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E71" s="3">
         <v>1</v>
@@ -4810,34 +4809,34 @@
         <v>14</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="J71" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="K71" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="L71" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="K71" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="L71" s="4" t="s">
-        <v>263</v>
       </c>
       <c r="M71" s="3"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C72" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="E72" s="3">
         <v>0</v>
@@ -4867,16 +4866,16 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E73" s="3">
         <v>0</v>
@@ -4906,16 +4905,16 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E74" s="3">
         <v>0</v>
@@ -4942,21 +4941,21 @@
         <v>-1</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
@@ -4983,21 +4982,21 @@
         <v>-1</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C76" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="E76" s="3">
         <v>1</v>
@@ -5009,16 +5008,16 @@
         <v>17</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I76" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J76" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="K76" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="L76" s="4">
         <v>33</v>
@@ -5027,13 +5026,13 @@
     </row>
     <row r="77" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3">
@@ -5046,16 +5045,16 @@
         <v>17</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I77" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J77" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="K77" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>176</v>
       </c>
       <c r="L77" s="4">
         <v>34</v>
@@ -5064,16 +5063,16 @@
     </row>
     <row r="78" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C78" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="E78" s="3">
         <v>1</v>
@@ -5085,16 +5084,16 @@
         <v>3</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I78" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J78" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>176</v>
       </c>
       <c r="L78" s="4">
         <v>38</v>
@@ -5103,16 +5102,16 @@
     </row>
     <row r="79" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="E79" s="3">
         <v>1</v>
@@ -5124,16 +5123,16 @@
         <v>14</v>
       </c>
       <c r="H79" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J79" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="I79" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J79" s="6" t="s">
+      <c r="K79" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="K79" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="L79" s="4">
         <v>30</v>
@@ -5142,16 +5141,16 @@
     </row>
     <row r="80" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C80" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="E80" s="3">
         <v>1</v>
@@ -5163,16 +5162,16 @@
         <v>14</v>
       </c>
       <c r="H80" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J80" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="I80" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J80" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="K80" s="6" t="s">
-        <v>175</v>
+      <c r="K80" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="L80" s="4">
         <v>31</v>
@@ -5181,16 +5180,16 @@
     </row>
     <row r="81" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C81" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="E81" s="3">
         <v>1</v>
@@ -5202,16 +5201,16 @@
         <v>3</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="J81" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="K81" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="K81" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="L81" s="4">
         <v>45</v>
@@ -5220,16 +5219,16 @@
     </row>
     <row r="82" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C82" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="E82" s="3">
         <v>1</v>
@@ -5241,32 +5240,32 @@
         <v>3</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="J82" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="K82" s="7"/>
+        <v>292</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="K82" s="6"/>
       <c r="L82" s="4">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="M82" s="3"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C83" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="E83" s="3">
         <v>0</v>
@@ -5296,16 +5295,16 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C84" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
@@ -5335,16 +5334,16 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C85" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="E85" s="3">
         <v>0</v>
@@ -5374,16 +5373,16 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C86" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="E86" s="3">
         <v>0</v>
@@ -5413,16 +5412,16 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E87" s="3">
         <v>0</v>
@@ -5452,16 +5451,16 @@
     </row>
     <row r="88" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C88" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="E88" s="3">
         <v>1</v>
@@ -5473,15 +5472,15 @@
         <v>14</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="I88" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="J88" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="I88" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="J88" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K88" s="11"/>
+      <c r="K88" s="10"/>
       <c r="L88" s="4">
         <v>32</v>
       </c>
@@ -5489,16 +5488,16 @@
     </row>
     <row r="89" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C89" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
@@ -5510,15 +5509,15 @@
         <v>14</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="I89" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="J89" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="J89" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="K89" s="11"/>
+      <c r="K89" s="10"/>
       <c r="L89" s="4">
         <v>23</v>
       </c>
@@ -5526,16 +5525,16 @@
     </row>
     <row r="90" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E90" s="3">
         <v>1</v>
@@ -5547,15 +5546,15 @@
         <v>14</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="I90" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="J90" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="K90" s="11"/>
+        <v>269</v>
+      </c>
+      <c r="I90" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="J90" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="K90" s="10"/>
       <c r="L90" s="4">
         <v>27</v>
       </c>
@@ -5563,16 +5562,16 @@
     </row>
     <row r="91" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C91" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="E91" s="3">
         <v>1</v>
@@ -5584,15 +5583,15 @@
         <v>14</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="I91" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="J91" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="K91" s="11"/>
+        <v>269</v>
+      </c>
+      <c r="I91" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="J91" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="K91" s="10"/>
       <c r="L91" s="4">
         <v>31</v>
       </c>
@@ -5600,16 +5599,16 @@
     </row>
     <row r="92" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C92" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="E92" s="3">
         <v>1</v>
@@ -5623,32 +5622,32 @@
       <c r="H92" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I92" s="8" t="s">
-        <v>294</v>
+      <c r="I92" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M92" s="3"/>
     </row>
     <row r="93" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E93" s="3">
         <v>1</v>
@@ -5662,32 +5661,32 @@
       <c r="H93" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I93" s="8" t="s">
-        <v>294</v>
+      <c r="I93" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L93" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M93" s="3"/>
     </row>
     <row r="94" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E94" s="3">
         <v>1</v>
@@ -5701,13 +5700,13 @@
       <c r="H94" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I94" s="8" t="s">
-        <v>294</v>
+      <c r="I94" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="K94" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="K94" s="8" t="s">
         <v>33</v>
       </c>
       <c r="L94" s="4">
@@ -5717,16 +5716,16 @@
     </row>
     <row r="95" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C95" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="E95" s="3">
         <v>1</v>
@@ -5740,13 +5739,13 @@
       <c r="H95" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I95" s="8" t="s">
-        <v>294</v>
+      <c r="I95" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="K95" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="K95" s="8" t="s">
         <v>33</v>
       </c>
       <c r="L95" s="4">
@@ -5756,16 +5755,16 @@
     </row>
     <row r="96" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E96" s="3">
         <v>1</v>
@@ -5779,13 +5778,13 @@
       <c r="H96" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I96" s="8" t="s">
-        <v>294</v>
+      <c r="I96" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="K96" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="K96" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L96" s="4">
@@ -5795,16 +5794,16 @@
     </row>
     <row r="97" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C97" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="E97" s="3">
         <v>1</v>
@@ -5818,13 +5817,13 @@
       <c r="H97" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I97" s="8" t="s">
-        <v>294</v>
+      <c r="I97" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="K97" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="K97" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L97" s="4">
@@ -5857,13 +5856,13 @@
       <c r="H98" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I98" s="8" t="s">
-        <v>294</v>
+      <c r="I98" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="J98" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K98" s="9" t="s">
+      <c r="K98" s="8" t="s">
         <v>41</v>
       </c>
       <c r="L98" s="4" t="s">
@@ -5896,8 +5895,8 @@
       <c r="H99" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I99" s="14" t="s">
-        <v>307</v>
+      <c r="I99" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J99" s="3" t="s">
         <v>47</v>
@@ -5935,13 +5934,13 @@
       <c r="H100" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I100" s="14" t="s">
-        <v>307</v>
+      <c r="I100" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J100" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K100" s="9" t="s">
+      <c r="K100" s="8" t="s">
         <v>59</v>
       </c>
       <c r="L100" s="4">
@@ -5974,13 +5973,13 @@
       <c r="H101" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I101" s="14" t="s">
-        <v>307</v>
+      <c r="I101" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J101" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K101" s="9" t="s">
+      <c r="K101" s="8" t="s">
         <v>46</v>
       </c>
       <c r="L101" s="4">
@@ -6013,13 +6012,13 @@
       <c r="H102" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I102" s="14" t="s">
-        <v>307</v>
+      <c r="I102" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J102" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K102" s="9" t="s">
+      <c r="K102" s="8" t="s">
         <v>54</v>
       </c>
       <c r="L102" s="4" t="s">
@@ -6052,13 +6051,13 @@
       <c r="H103" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I103" s="14" t="s">
-        <v>307</v>
+      <c r="I103" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J103" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K103" s="9" t="s">
+      <c r="K103" s="8" t="s">
         <v>67</v>
       </c>
       <c r="L103" s="4" t="s">
@@ -6091,8 +6090,8 @@
       <c r="H104" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I104" s="14" t="s">
-        <v>307</v>
+      <c r="I104" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J104" s="3" t="s">
         <v>47</v>
@@ -6130,8 +6129,8 @@
       <c r="H105" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I105" s="14" t="s">
-        <v>308</v>
+      <c r="I105" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>47</v>
@@ -6169,13 +6168,13 @@
       <c r="H106" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I106" s="14" t="s">
-        <v>307</v>
+      <c r="I106" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J106" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K106" s="9" t="s">
+      <c r="K106" s="8" t="s">
         <v>59</v>
       </c>
       <c r="L106" s="4">
@@ -6208,13 +6207,13 @@
       <c r="H107" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I107" s="14" t="s">
-        <v>308</v>
+      <c r="I107" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="J107" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K107" s="9" t="s">
+      <c r="K107" s="8" t="s">
         <v>46</v>
       </c>
       <c r="L107" s="4">
@@ -6247,13 +6246,13 @@
       <c r="H108" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I108" s="14" t="s">
-        <v>308</v>
+      <c r="I108" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="J108" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K108" s="9" t="s">
+      <c r="K108" s="8" t="s">
         <v>54</v>
       </c>
       <c r="L108" s="4" t="s">
@@ -6286,13 +6285,13 @@
       <c r="H109" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I109" s="14" t="s">
-        <v>308</v>
+      <c r="I109" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="J109" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K109" s="9" t="s">
+      <c r="K109" s="8" t="s">
         <v>67</v>
       </c>
       <c r="L109" s="4" t="s">
@@ -6325,8 +6324,8 @@
       <c r="H110" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I110" s="14" t="s">
-        <v>308</v>
+      <c r="I110" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="J110" s="3" t="s">
         <v>47</v>
@@ -6341,16 +6340,16 @@
     </row>
     <row r="111" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C111" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="E111" s="3">
         <v>1</v>
@@ -6362,32 +6361,32 @@
         <v>14</v>
       </c>
       <c r="H111" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="K111" s="10"/>
+      <c r="L111" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="I111" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="J111" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="K111" s="11"/>
-      <c r="L111" s="4" t="s">
-        <v>291</v>
       </c>
       <c r="M111" s="3"/>
     </row>
     <row r="112" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E112" s="3">
         <v>1</v>
@@ -6399,15 +6398,15 @@
         <v>14</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="K112" s="11"/>
+        <v>309</v>
+      </c>
+      <c r="K112" s="10"/>
       <c r="L112" s="4">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
updated SIT emission map to remove duplicate field
</commit_message>
<xml_diff>
--- a/sisepuede/ref/data_crosswalks/sisepuede_fields_to_epa_state_inventory_tool_emissions_map.xlsx
+++ b/sisepuede/ref/data_crosswalks/sisepuede_fields_to_epa_state_inventory_tool_emissions_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/data_crosswalks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5B3359-F60F-094A-9B32-F3129DEEBAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38FEFC2-8BA4-C548-91D2-823054729F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="760" windowWidth="33420" windowHeight="18280" activeTab="1" xr2:uid="{9DBDAEDA-F5AA-E443-9947-E206192A213F}"/>
+    <workbookView xWindow="1220" yWindow="760" windowWidth="33420" windowHeight="18280" activeTab="1" xr2:uid="{9DBDAEDA-F5AA-E443-9947-E206192A213F}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="310">
   <si>
     <t>NA</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>co2</t>
-  </si>
-  <si>
-    <t>emission_co2e_co2_fgtv_fuel_natural_gas</t>
   </si>
   <si>
     <t>emission_co2e_co2_fgtv_fuel_coal</t>
@@ -1982,53 +1979,53 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
         <v>118</v>
-      </c>
-      <c r="C4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
         <v>122</v>
-      </c>
-      <c r="C6" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2038,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9645CE76-D122-B846-99B1-A3A394E64618}">
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:M111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2057,78 +2054,78 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L2" s="4">
         <v>35</v>
@@ -2137,37 +2134,37 @@
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L3" s="4">
         <v>36</v>
@@ -2176,37 +2173,37 @@
     </row>
     <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L4" s="4">
         <v>40</v>
@@ -2215,16 +2212,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -2254,16 +2251,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -2293,16 +2290,16 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -2332,16 +2329,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -2371,16 +2368,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -2410,37 +2407,37 @@
     </row>
     <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L10" s="4">
         <v>46</v>
@@ -2449,16 +2446,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -2488,16 +2485,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -2527,16 +2524,16 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
@@ -2566,37 +2563,37 @@
     </row>
     <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L14" s="4">
         <v>28</v>
@@ -2605,37 +2602,37 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L15" s="4">
         <v>25</v>
@@ -2644,37 +2641,37 @@
     </row>
     <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L16" s="4">
         <v>27</v>
@@ -2683,37 +2680,37 @@
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L17" s="4">
         <v>26</v>
@@ -2722,37 +2719,37 @@
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="K18" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L18" s="4">
         <v>11</v>
@@ -2761,16 +2758,16 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -2800,16 +2797,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -2839,16 +2836,16 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
@@ -2878,16 +2875,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -2917,16 +2914,16 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
@@ -2956,16 +2953,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -2995,16 +2992,16 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -3034,16 +3031,16 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
@@ -3073,16 +3070,16 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
@@ -3112,37 +3109,37 @@
     </row>
     <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L28" s="4">
         <v>15</v>
@@ -3151,37 +3148,37 @@
     </row>
     <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" s="3">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L29" s="4">
         <v>14</v>
@@ -3190,34 +3187,34 @@
     </row>
     <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="4">
@@ -3227,34 +3224,34 @@
     </row>
     <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="J31" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="4">
@@ -3264,34 +3261,34 @@
     </row>
     <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E32" s="3">
         <v>1</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="4">
@@ -3301,34 +3298,34 @@
     </row>
     <row r="33" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="4">
@@ -3338,74 +3335,74 @@
     </row>
     <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" s="3">
         <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K34" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="L34" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L35" s="4">
         <v>12</v>
@@ -3414,35 +3411,35 @@
     </row>
     <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" s="3">
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L36" s="4">
         <v>11</v>
@@ -3451,37 +3448,37 @@
     </row>
     <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H37" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="J37" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>232</v>
-      </c>
       <c r="K37" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L37" s="4">
         <v>27</v>
@@ -3490,55 +3487,55 @@
     </row>
     <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H38" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="J38" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="J38" s="8" t="s">
+      <c r="K38" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="L38" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
@@ -3568,16 +3565,16 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
@@ -3607,16 +3604,16 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
@@ -3646,16 +3643,16 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
@@ -3691,7 +3688,7 @@
         <v>9</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>7</v>
@@ -3730,7 +3727,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
@@ -3766,13 +3763,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
@@ -3808,7 +3805,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>1</v>
@@ -3847,7 +3844,7 @@
         <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>1</v>
@@ -3878,291 +3875,291 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>2</v>
+        <v>157</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" s="3">
         <v>1</v>
       </c>
-      <c r="E48" s="3">
-        <v>0</v>
-      </c>
       <c r="F48" s="3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>0</v>
+        <v>109</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>0</v>
+        <v>291</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L48" s="4">
-        <v>-1</v>
+        <v>160</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="M48" s="3"/>
     </row>
     <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D49" s="3" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="E49" s="3">
         <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H49" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="J49" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I49" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="L49" s="4" t="s">
-        <v>167</v>
+      <c r="K49" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L49" s="4">
+        <v>5</v>
       </c>
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="E50" s="3">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="J50" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="K50" s="8" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="L50" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M50" s="3"/>
     </row>
     <row r="51" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E51" s="3">
         <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H51" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="J51" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I51" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="K51" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L51" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M51" s="3"/>
     </row>
     <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="J52" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I52" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="K52" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="L52" s="4">
-        <v>6</v>
+        <v>292</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="M52" s="3"/>
     </row>
     <row r="53" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H53" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="J53" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I53" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="K53" s="8" t="s">
-        <v>293</v>
+        <v>143</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="E54" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I54" s="7" t="s">
-        <v>288</v>
+        <v>0</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K54" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="L54" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54" s="4">
+        <v>-1</v>
       </c>
       <c r="M54" s="3"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E55" s="3">
         <v>0</v>
@@ -4192,16 +4189,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>164</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E56" s="3">
         <v>0</v>
@@ -4231,16 +4228,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>165</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
@@ -4270,16 +4267,16 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
@@ -4309,16 +4306,16 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="E59" s="3">
         <v>0</v>
@@ -4348,7 +4345,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>9</v>
@@ -4357,7 +4354,7 @@
         <v>148</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E60" s="3">
         <v>0</v>
@@ -4387,7 +4384,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>9</v>
@@ -4396,7 +4393,7 @@
         <v>149</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E61" s="3">
         <v>0</v>
@@ -4426,7 +4423,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>9</v>
@@ -4435,7 +4432,7 @@
         <v>150</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E62" s="3">
         <v>0</v>
@@ -4465,7 +4462,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>9</v>
@@ -4474,7 +4471,7 @@
         <v>151</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E63" s="3">
         <v>0</v>
@@ -4504,7 +4501,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>9</v>
@@ -4513,7 +4510,7 @@
         <v>152</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E64" s="3">
         <v>0</v>
@@ -4543,7 +4540,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>9</v>
@@ -4552,7 +4549,7 @@
         <v>153</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E65" s="3">
         <v>0</v>
@@ -4582,16 +4579,16 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E66" s="3">
         <v>0</v>
@@ -4621,7 +4618,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>3</v>
@@ -4630,7 +4627,7 @@
         <v>155</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E67" s="3">
         <v>0</v>
@@ -4660,7 +4657,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>3</v>
@@ -4669,7 +4666,7 @@
         <v>156</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E68" s="3">
         <v>0</v>
@@ -4697,133 +4694,133 @@
       </c>
       <c r="M68" s="3"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>132</v>
+        <v>242</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>157</v>
+        <v>241</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>143</v>
+        <v>243</v>
       </c>
       <c r="E69" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>0</v>
+        <v>290</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="K69" s="10"/>
       <c r="L69" s="4">
-        <v>-1</v>
+        <v>40</v>
       </c>
       <c r="M69" s="3"/>
     </row>
     <row r="70" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E70" s="3">
         <v>1</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="K70" s="10"/>
-      <c r="L70" s="4">
-        <v>40</v>
+        <v>290</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="K70" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="M70" s="3"/>
     </row>
-    <row r="71" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E71" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>231</v>
+        <v>0</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="K71" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="L71" s="4" t="s">
-        <v>256</v>
+        <v>0</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L71" s="4">
+        <v>-1</v>
       </c>
       <c r="M71" s="3"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="E72" s="3">
         <v>0</v>
@@ -4853,16 +4850,16 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E73" s="3">
         <v>0</v>
@@ -4888,20 +4885,22 @@
       <c r="L73" s="4">
         <v>-1</v>
       </c>
-      <c r="M73" s="3"/>
+      <c r="M73" s="3" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E74" s="3">
         <v>0</v>
@@ -4928,123 +4927,121 @@
         <v>-1</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>243</v>
+        <v>181</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>250</v>
+        <v>179</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>251</v>
+        <v>180</v>
       </c>
       <c r="E75" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="L75" s="4">
-        <v>-1</v>
-      </c>
-      <c r="M75" s="3" t="s">
-        <v>253</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="M75" s="3"/>
     </row>
     <row r="76" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>181</v>
-      </c>
+      <c r="D76" s="3"/>
       <c r="E76" s="3">
         <v>1</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>172</v>
       </c>
       <c r="L76" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M76" s="3"/>
     </row>
     <row r="77" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D77" s="3"/>
+        <v>309</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="E77" s="3">
         <v>1</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L77" s="4">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M77" s="3"/>
     </row>
@@ -5053,206 +5050,206 @@
         <v>185</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>310</v>
+        <v>188</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E78" s="3">
         <v>1</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H78" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="J78" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="I78" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="J78" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="K78" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L78" s="4">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="M78" s="3"/>
     </row>
     <row r="79" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E79" s="3">
         <v>1</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H79" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="J79" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="J79" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="K79" s="5" t="s">
         <v>170</v>
       </c>
       <c r="L79" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M79" s="3"/>
     </row>
     <row r="80" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E80" s="3">
         <v>1</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I80" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="I80" s="3" t="s">
         <v>285</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="K80" s="5" t="s">
-        <v>171</v>
+        <v>200</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="L80" s="4">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="M80" s="3"/>
     </row>
     <row r="81" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="E81" s="3">
         <v>1</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="K81" s="6" t="s">
         <v>202</v>
       </c>
+      <c r="K81" s="6"/>
       <c r="L81" s="4">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="M81" s="3"/>
     </row>
-    <row r="82" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="E82" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J82" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="K82" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K82" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="L82" s="4">
-        <v>51</v>
+        <v>-1</v>
       </c>
       <c r="M82" s="3"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>186</v>
+        <v>261</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>226</v>
+        <v>265</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>227</v>
+        <v>266</v>
       </c>
       <c r="E83" s="3">
         <v>0</v>
@@ -5282,16 +5279,16 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
@@ -5321,16 +5318,16 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E85" s="3">
         <v>0</v>
@@ -5360,16 +5357,16 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E86" s="3">
         <v>0</v>
@@ -5397,1013 +5394,974 @@
       </c>
       <c r="M86" s="3"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E87" s="3">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H87" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E87" s="3">
-        <v>0</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K87" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="I87" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="J87" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K87" s="10"/>
       <c r="L87" s="4">
-        <v>-1</v>
+        <v>32</v>
       </c>
       <c r="M87" s="3"/>
     </row>
     <row r="88" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="E88" s="3">
         <v>1</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="I88" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="I88" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="J88" s="8" t="s">
-        <v>33</v>
+      <c r="J88" s="11" t="s">
+        <v>295</v>
       </c>
       <c r="K88" s="10"/>
       <c r="L88" s="4">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="M88" s="3"/>
     </row>
     <row r="89" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="I89" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="J89" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="I89" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="J89" s="12" t="s">
         <v>296</v>
       </c>
       <c r="K89" s="10"/>
       <c r="L89" s="4">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M89" s="3"/>
     </row>
     <row r="90" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E90" s="3">
         <v>1</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J90" s="12" t="s">
         <v>297</v>
       </c>
       <c r="K90" s="10"/>
       <c r="L90" s="4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="M90" s="3"/>
     </row>
     <row r="91" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>276</v>
+        <v>221</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>277</v>
+        <v>222</v>
       </c>
       <c r="E91" s="3">
         <v>1</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="I91" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="J91" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="K91" s="10"/>
-      <c r="L91" s="4">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L91" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="M91" s="3"/>
     </row>
     <row r="92" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C92" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="E92" s="3">
         <v>1</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I92" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M92" s="3"/>
     </row>
     <row r="93" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E93" s="3">
         <v>1</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="K93" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L93" s="4" t="s">
-        <v>224</v>
+        <v>218</v>
+      </c>
+      <c r="K93" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L93" s="4">
+        <v>9</v>
       </c>
       <c r="M93" s="3"/>
     </row>
     <row r="94" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E94" s="3">
         <v>1</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="K94" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L94" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M94" s="3"/>
     </row>
     <row r="95" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E95" s="3">
         <v>1</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I95" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="K95" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L95" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M95" s="3"/>
     </row>
     <row r="96" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E96" s="3">
         <v>1</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="K96" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L96" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M96" s="3"/>
     </row>
     <row r="97" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>213</v>
+        <v>43</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>214</v>
+        <v>42</v>
       </c>
       <c r="E97" s="3">
         <v>1</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I97" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>212</v>
+        <v>41</v>
       </c>
       <c r="K97" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L97" s="4">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="L97" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="M97" s="3"/>
     </row>
     <row r="98" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E98" s="3">
         <v>1</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I98" s="7" t="s">
-        <v>287</v>
+        <v>47</v>
+      </c>
+      <c r="I98" s="13" t="s">
+        <v>298</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K98" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L98" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L98" s="4">
+        <v>73</v>
       </c>
       <c r="M98" s="3"/>
     </row>
     <row r="99" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E99" s="3">
         <v>1</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I99" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K99" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="K99" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="L99" s="4">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="M99" s="3"/>
     </row>
     <row r="100" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E100" s="3">
         <v>1</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I100" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K100" s="8" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="L100" s="4">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="M100" s="3"/>
     </row>
     <row r="101" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E101" s="3">
         <v>1</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I101" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K101" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L101" s="4">
-        <v>70</v>
+        <v>53</v>
+      </c>
+      <c r="L101" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="M101" s="3"/>
     </row>
     <row r="102" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E102" s="3">
         <v>1</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I102" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K102" s="8" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="L102" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="M102" s="3"/>
     </row>
     <row r="103" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E103" s="3">
         <v>1</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I103" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K103" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="L103" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L103" s="4">
         <v>69</v>
       </c>
       <c r="M103" s="3"/>
     </row>
     <row r="104" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E104" s="3">
         <v>1</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I104" s="13" t="s">
         <v>299</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="L104" s="4">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="M104" s="3"/>
     </row>
     <row r="105" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E105" s="3">
         <v>1</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I105" s="13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K105" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="K105" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="L105" s="4">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="M105" s="3"/>
     </row>
     <row r="106" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E106" s="3">
         <v>1</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I106" s="13" t="s">
         <v>299</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K106" s="8" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="L106" s="4">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="M106" s="3"/>
     </row>
     <row r="107" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E107" s="3">
         <v>1</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I107" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K107" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="L107" s="4">
-        <v>98</v>
+        <v>53</v>
+      </c>
+      <c r="L107" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="M107" s="3"/>
     </row>
     <row r="108" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E108" s="3">
         <v>1</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I108" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K108" s="8" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="L108" s="4" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="M108" s="3"/>
     </row>
     <row r="109" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E109" s="3">
         <v>1</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I109" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K109" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="L109" s="4" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="K109" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L109" s="4">
+        <v>97</v>
       </c>
       <c r="M109" s="3"/>
     </row>
     <row r="110" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>73</v>
+        <v>277</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>49</v>
+        <v>278</v>
       </c>
       <c r="E110" s="3">
         <v>1</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I110" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="J110" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="J110" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K110" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="L110" s="4">
-        <v>97</v>
+      <c r="K110" s="10"/>
+      <c r="L110" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="M110" s="3"/>
     </row>
     <row r="111" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="E111" s="3">
         <v>1</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J111" s="3" t="s">
         <v>301</v>
       </c>
       <c r="K111" s="10"/>
-      <c r="L111" s="4" t="s">
-        <v>284</v>
+      <c r="L111" s="4">
+        <v>6</v>
       </c>
       <c r="M111" s="3"/>
     </row>
-    <row r="112" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E112" s="3">
-        <v>1</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H112" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="J112" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="K112" s="10"/>
-      <c r="L112" s="4">
-        <v>6</v>
-      </c>
-      <c r="M112" s="3"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M112">
-    <sortCondition ref="A2:A112"/>
-    <sortCondition ref="H2:H112"/>
-    <sortCondition ref="C2:C112"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M111">
+    <sortCondition ref="A2:A111"/>
+    <sortCondition ref="H2:H111"/>
+    <sortCondition ref="C2:C111"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated emission map for EPA SIT
</commit_message>
<xml_diff>
--- a/sisepuede/ref/data_crosswalks/sisepuede_fields_to_epa_state_inventory_tool_emissions_map.xlsx
+++ b/sisepuede/ref/data_crosswalks/sisepuede_fields_to_epa_state_inventory_tool_emissions_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/data_crosswalks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB1ACA0-2793-0043-B476-C51ACA14EC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3328CE0-FBC9-3642-9088-40E07DCD6217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="760" windowWidth="33900" windowHeight="20100" activeTab="1" xr2:uid="{9DBDAEDA-F5AA-E443-9947-E206192A213F}"/>
+    <workbookView xWindow="360" yWindow="760" windowWidth="33900" windowHeight="20100" activeTab="1" xr2:uid="{9DBDAEDA-F5AA-E443-9947-E206192A213F}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -1999,7 +1999,7 @@
   <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>